<commit_message>
added papers to source tab
</commit_message>
<xml_diff>
--- a/data/ospree_newpapers.xlsx
+++ b/data/ospree_newpapers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/ospree/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9949F8FF-4938-4A49-8042-F860794BE110}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385AF87D-206F-0D4A-A568-325F436EC144}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13640" yWindow="4360" windowWidth="34900" windowHeight="16940" xr2:uid="{2FD8B3AA-A0EB-3D46-9BA6-4DB5E6E588DB}"/>
+    <workbookView xWindow="26020" yWindow="880" windowWidth="34900" windowHeight="16940" activeTab="1" xr2:uid="{2FD8B3AA-A0EB-3D46-9BA6-4DB5E6E588DB}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="data_detailed" sheetId="1" r:id="rId4"/>
     <sheet name="scratch" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="311">
   <si>
     <t>datasetID</t>
   </si>
@@ -810,6 +810,210 @@
   </si>
   <si>
     <t>Main data sheet. Response variables</t>
+  </si>
+  <si>
+    <t>Fu_et_al_2019.pdf</t>
+  </si>
+  <si>
+    <t>Yongshuo H. Fu, Shilong Piao, Xuancheng Zhou,  Xiaojun Geng, Fanghua Hao, Yann Vitasse, Ivan A. Janssens</t>
+  </si>
+  <si>
+    <t>Short photoperiod reduces temperature sensitivity of leaf-out in saplings of Fagus sylvatica bud not in horse chestnut</t>
+  </si>
+  <si>
+    <t>Global Change Biology</t>
+  </si>
+  <si>
+    <t>1696-1703</t>
+  </si>
+  <si>
+    <t>man17</t>
+  </si>
+  <si>
+    <t>fu19</t>
+  </si>
+  <si>
+    <t>richardson18</t>
+  </si>
+  <si>
+    <t>vitra17</t>
+  </si>
+  <si>
+    <t>prevey18</t>
+  </si>
+  <si>
+    <t>flynn18</t>
+  </si>
+  <si>
+    <t>malyshev18</t>
+  </si>
+  <si>
+    <t>nanninga17</t>
+  </si>
+  <si>
+    <t>anzanello16</t>
+  </si>
+  <si>
+    <t>anzanello18</t>
+  </si>
+  <si>
+    <t>ramos17</t>
+  </si>
+  <si>
+    <t>D. F. B. Flynn &amp; E. M. Wolkovich</t>
+  </si>
+  <si>
+    <t>Temperature and photoperiod drive spring phenology across all species in a temperate forest community</t>
+  </si>
+  <si>
+    <t>New Phytologist</t>
+  </si>
+  <si>
+    <t>1353-1362</t>
+  </si>
+  <si>
+    <t>fu18</t>
+  </si>
+  <si>
+    <t>Fu_et_al-2018-Global_Change_Biology.pdf</t>
+  </si>
+  <si>
+    <t>Flynn_et_al-2018-New_Phytologist.pdf</t>
+  </si>
+  <si>
+    <t>Yongshuo H. Fu, Shilong Piao, Nicolas Delpierre, Fanghua Hao, Heikki H€anninen, Yongjie Liu, Wenchao Sun, Ivan A. Janssens, Matteo Campioli</t>
+  </si>
+  <si>
+    <t>Larger temperature response of autumn leaf senescence than spring leaf-out phenology</t>
+  </si>
+  <si>
+    <t>2159-2168</t>
+  </si>
+  <si>
+    <t>Ramos et al. 2018.pdf</t>
+  </si>
+  <si>
+    <t>A. Ramos, H.F. Rapoport, D. Cabello, L. Rallo</t>
+  </si>
+  <si>
+    <t>Chilling accumulation, dormancy release temperature, and the role of leaves in olive reproductive budburst: Evaluation using shoot explants</t>
+  </si>
+  <si>
+    <t>Scientia Horticulturae</t>
+  </si>
+  <si>
+    <t>241-252</t>
+  </si>
+  <si>
+    <t>Malyshev et al. 2018.pdf</t>
+  </si>
+  <si>
+    <t>Andrey V. Malyshev, Hugh A.L. Henry, Andreas Bolte, Mohammed A.S. Arfin Khan,  Juergen Kreyling</t>
+  </si>
+  <si>
+    <t>Temporal photoperiod sensitivity and forcing requirements for budburst in temperate tree seedlings</t>
+  </si>
+  <si>
+    <t>Agriculutural and Forest Meteorology</t>
+  </si>
+  <si>
+    <t>82-90</t>
+  </si>
+  <si>
+    <t>Man et al. 2017.pdf</t>
+  </si>
+  <si>
+    <t>Rongzhou Man, Pengxin Lu, Qing-Lai Dang</t>
+  </si>
+  <si>
+    <t>Insufficient chilling effects vary among boreal tree species and chilling duration</t>
+  </si>
+  <si>
+    <t>Frontiers in Plant Science</t>
+  </si>
+  <si>
+    <t>Anzanello &amp; Biasi 20186.pdf</t>
+  </si>
+  <si>
+    <t>Rafael Anzanello, Luiz Antonio Biasi</t>
+  </si>
+  <si>
+    <t>Base temperature as a function of genotype: a foundation for modeling phenology of temperate fruit species</t>
+  </si>
+  <si>
+    <t>Semina: Ciencias Agrarias</t>
+  </si>
+  <si>
+    <t>1811-1826</t>
+  </si>
+  <si>
+    <t>Anzanello et al. 2018.pdf</t>
+  </si>
+  <si>
+    <t>Rafael Anzanello, Flavio Bello Fialho, Henrique Pessoa dos Santos</t>
+  </si>
+  <si>
+    <t>Chilling requirements and dormancy evolution in grapevine buds</t>
+  </si>
+  <si>
+    <t>Ciencia e Agrotecnologia</t>
+  </si>
+  <si>
+    <t>364-371</t>
+  </si>
+  <si>
+    <t>prevey &amp; Harrington 2019.pdf</t>
+  </si>
+  <si>
+    <t>Janet S. Prevey and Constance A. Harrington</t>
+  </si>
+  <si>
+    <t>Effectiveness of winter temperatures for satisfying chilling requirements for reproductive budburst of red alder (Alnus rubra)</t>
+  </si>
+  <si>
+    <t>PeerJ</t>
+  </si>
+  <si>
+    <t>Nanninga et al. 2017.pdf</t>
+  </si>
+  <si>
+    <t>Claudia Nanninga, Chris R. Buyarski, Andrew M. Pretorius, Rebecca A. Montegomery</t>
+  </si>
+  <si>
+    <t>Increased exposure to chilling advances the time to budburst in North American tree species</t>
+  </si>
+  <si>
+    <t>Tree Physiology</t>
+  </si>
+  <si>
+    <t>1727-1738</t>
+  </si>
+  <si>
+    <t>Vitra_et_al-2017.pdf</t>
+  </si>
+  <si>
+    <t>Amarante Vitra, Armando Lenz, Yann Vitasse</t>
+  </si>
+  <si>
+    <t>Frost hardening and dehardening potential in temperate trees from winter to budburst</t>
+  </si>
+  <si>
+    <t>113-123</t>
+  </si>
+  <si>
+    <t>Richardson et al. 2018.pdf</t>
+  </si>
+  <si>
+    <t>Richardson, Andrew D. and Hufkens, Koen and Milliman, Thomas and Aubrecht, Donald M. and Furze, Morgan E. and Seyednasrollah, Bijan and Krassovski, Misha B. and Latimer, John M. and Nettles, W. Robert and Heiderman, Ryan R. and Warren, Jeffrey M. and Hanson, Paul J.</t>
+  </si>
+  <si>
+    <t>Ecosystem warming extends vegetation activity but heightens vulnerability to cold temperatures</t>
+  </si>
+  <si>
+    <t>Nature</t>
+  </si>
+  <si>
+    <t>368-371</t>
   </si>
 </sst>
 </file>
@@ -898,7 +1102,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -914,12 +1118,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -931,12 +1129,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1293,7 +1501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69779EF-BC31-6940-ABCF-A12C8E53378E}">
   <dimension ref="A1:P160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
@@ -1339,7 +1547,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="3"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="10"/>
+      <c r="K7" s="8"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
@@ -1438,45 +1646,45 @@
       <c r="A19" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="9" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D20" s="11"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="D21" s="11"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D22" s="11"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="9" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1484,7 +1692,7 @@
       <c r="A24" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="9" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1492,7 +1700,7 @@
       <c r="A25" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="9" t="s">
         <v>187</v>
       </c>
     </row>
@@ -1780,7 +1988,7 @@
       <c r="B66" t="s">
         <v>221</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="15" t="s">
         <v>222</v>
       </c>
     </row>
@@ -1791,7 +1999,7 @@
       <c r="B67" t="s">
         <v>113</v>
       </c>
-      <c r="C67" s="7"/>
+      <c r="C67" s="15"/>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
@@ -1864,7 +2072,7 @@
       <c r="B76" t="s">
         <v>237</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="15" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1875,7 +2083,7 @@
       <c r="B77" t="s">
         <v>120</v>
       </c>
-      <c r="C77" s="7"/>
+      <c r="C77" s="15"/>
     </row>
     <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
@@ -1884,7 +2092,7 @@
       <c r="B78" t="s">
         <v>122</v>
       </c>
-      <c r="C78" s="7"/>
+      <c r="C78" s="15"/>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
@@ -1893,7 +2101,7 @@
       <c r="B79" t="s">
         <v>124</v>
       </c>
-      <c r="C79" s="7"/>
+      <c r="C79" s="15"/>
     </row>
     <row r="80" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
@@ -1902,7 +2110,7 @@
       <c r="B80" t="s">
         <v>126</v>
       </c>
-      <c r="C80" s="7"/>
+      <c r="C80" s="15"/>
     </row>
     <row r="81" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
@@ -2151,7 +2359,7 @@
       <c r="B114" t="s">
         <v>83</v>
       </c>
-      <c r="C114" s="7" t="s">
+      <c r="C114" s="15" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2162,7 +2370,7 @@
       <c r="B115" t="s">
         <v>86</v>
       </c>
-      <c r="C115" s="7"/>
+      <c r="C115" s="15"/>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
@@ -2203,7 +2411,7 @@
       <c r="B120" t="s">
         <v>94</v>
       </c>
-      <c r="C120" s="7" t="s">
+      <c r="C120" s="15" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2214,7 +2422,7 @@
       <c r="B121" t="s">
         <v>97</v>
       </c>
-      <c r="C121" s="7"/>
+      <c r="C121" s="15"/>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
@@ -2286,7 +2494,7 @@
       <c r="B131" t="s">
         <v>111</v>
       </c>
-      <c r="C131" s="7" t="s">
+      <c r="C131" s="15" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2297,7 +2505,7 @@
       <c r="B132" t="s">
         <v>113</v>
       </c>
-      <c r="C132" s="8"/>
+      <c r="C132" s="16"/>
     </row>
     <row r="133" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
@@ -2306,7 +2514,7 @@
       <c r="B133" t="s">
         <v>114</v>
       </c>
-      <c r="C133" s="8"/>
+      <c r="C133" s="16"/>
     </row>
     <row r="134" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
@@ -2315,7 +2523,7 @@
       <c r="B134" t="s">
         <v>115</v>
       </c>
-      <c r="C134" s="8"/>
+      <c r="C134" s="16"/>
     </row>
     <row r="135" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
@@ -2324,7 +2532,7 @@
       <c r="B135" t="s">
         <v>117</v>
       </c>
-      <c r="C135" s="7" t="s">
+      <c r="C135" s="15" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2335,7 +2543,7 @@
       <c r="B136" t="s">
         <v>120</v>
       </c>
-      <c r="C136" s="7"/>
+      <c r="C136" s="15"/>
     </row>
     <row r="137" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
@@ -2344,7 +2552,7 @@
       <c r="B137" t="s">
         <v>122</v>
       </c>
-      <c r="C137" s="7"/>
+      <c r="C137" s="15"/>
     </row>
     <row r="138" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
@@ -2353,7 +2561,7 @@
       <c r="B138" t="s">
         <v>124</v>
       </c>
-      <c r="C138" s="7"/>
+      <c r="C138" s="15"/>
     </row>
     <row r="139" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
@@ -2362,101 +2570,101 @@
       <c r="B139" t="s">
         <v>126</v>
       </c>
-      <c r="C139" s="7"/>
+      <c r="C139" s="15"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A142" s="12"/>
-      <c r="B142" s="13"/>
+      <c r="A142" s="10"/>
+      <c r="B142" s="11"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A143" s="13"/>
-      <c r="B143" s="13"/>
+      <c r="A143" s="11"/>
+      <c r="B143" s="11"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A144" s="13"/>
-      <c r="B144" s="13"/>
+      <c r="A144" s="11"/>
+      <c r="B144" s="11"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="12"/>
-      <c r="B145" s="13"/>
+      <c r="A145" s="10"/>
+      <c r="B145" s="11"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="14"/>
-      <c r="B146" s="13"/>
+      <c r="A146" s="12"/>
+      <c r="B146" s="11"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="12"/>
-      <c r="B147" s="13"/>
+      <c r="A147" s="10"/>
+      <c r="B147" s="11"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="12"/>
-      <c r="B148" s="13"/>
+      <c r="A148" s="10"/>
+      <c r="B148" s="11"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="12"/>
-      <c r="B149" s="13"/>
+      <c r="A149" s="10"/>
+      <c r="B149" s="11"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="12"/>
-      <c r="B150" s="13"/>
+      <c r="A150" s="10"/>
+      <c r="B150" s="11"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="12"/>
-      <c r="B151" s="13"/>
+      <c r="A151" s="10"/>
+      <c r="B151" s="11"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="15"/>
-      <c r="B152" s="15"/>
+      <c r="A152" s="17"/>
+      <c r="B152" s="17"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="16"/>
-      <c r="B153" s="17"/>
+      <c r="A153" s="13"/>
+      <c r="B153" s="14"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="12"/>
-      <c r="B154" s="13"/>
+      <c r="A154" s="10"/>
+      <c r="B154" s="11"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="12"/>
-      <c r="B155" s="13"/>
+      <c r="A155" s="10"/>
+      <c r="B155" s="11"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="12"/>
-      <c r="B156" s="13"/>
+      <c r="A156" s="10"/>
+      <c r="B156" s="11"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="12"/>
-      <c r="B157" s="13"/>
+      <c r="A157" s="10"/>
+      <c r="B157" s="11"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="12"/>
-      <c r="B158" s="13"/>
+      <c r="A158" s="10"/>
+      <c r="B158" s="11"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="12"/>
-      <c r="B159" s="13"/>
+      <c r="A159" s="10"/>
+      <c r="B159" s="11"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="12"/>
-      <c r="B160" s="13"/>
+      <c r="A160" s="10"/>
+      <c r="B160" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C76:C80"/>
     <mergeCell ref="C114:C115"/>
     <mergeCell ref="C120:C121"/>
     <mergeCell ref="C131:C134"/>
     <mergeCell ref="C135:C139"/>
     <mergeCell ref="A152:B152"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C76:C80"/>
   </mergeCells>
   <conditionalFormatting sqref="A7">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="3" priority="2">
       <formula>LEN(TRIM(A7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(A8))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2469,13 +2677,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2383E102-A742-244B-8C40-0636B840A46E}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
@@ -2536,14 +2747,318 @@
         <v>144</v>
       </c>
     </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2">
+        <v>2019</v>
+      </c>
+      <c r="E2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" t="s">
+        <v>280</v>
+      </c>
+      <c r="D3">
+        <v>2017</v>
+      </c>
+      <c r="E3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D4">
+        <v>2108</v>
+      </c>
+      <c r="E4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F4" t="s">
+        <v>309</v>
+      </c>
+      <c r="G4">
+        <v>560</v>
+      </c>
+      <c r="H4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5">
+        <v>2017</v>
+      </c>
+      <c r="E5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G5">
+        <v>216</v>
+      </c>
+      <c r="H5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D6">
+        <v>2018</v>
+      </c>
+      <c r="E6" t="s">
+        <v>295</v>
+      </c>
+      <c r="F6" t="s">
+        <v>296</v>
+      </c>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B7" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7">
+        <v>2018</v>
+      </c>
+      <c r="E7" t="s">
+        <v>260</v>
+      </c>
+      <c r="F7" t="s">
+        <v>261</v>
+      </c>
+      <c r="G7">
+        <v>219</v>
+      </c>
+      <c r="H7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D8">
+        <v>2018</v>
+      </c>
+      <c r="E8" t="s">
+        <v>276</v>
+      </c>
+      <c r="F8" t="s">
+        <v>277</v>
+      </c>
+      <c r="G8">
+        <v>248</v>
+      </c>
+      <c r="H8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B9" t="s">
+        <v>297</v>
+      </c>
+      <c r="C9" t="s">
+        <v>298</v>
+      </c>
+      <c r="D9">
+        <v>2017</v>
+      </c>
+      <c r="E9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F9" t="s">
+        <v>300</v>
+      </c>
+      <c r="G9">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C10" t="s">
+        <v>284</v>
+      </c>
+      <c r="D10">
+        <v>2016</v>
+      </c>
+      <c r="E10" t="s">
+        <v>285</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="G10">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>257</v>
+      </c>
+      <c r="B11" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11" t="s">
+        <v>289</v>
+      </c>
+      <c r="D11">
+        <v>2018</v>
+      </c>
+      <c r="E11" t="s">
+        <v>290</v>
+      </c>
+      <c r="F11" t="s">
+        <v>291</v>
+      </c>
+      <c r="G11">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" t="s">
+        <v>269</v>
+      </c>
+      <c r="C12" t="s">
+        <v>270</v>
+      </c>
+      <c r="D12">
+        <v>2018</v>
+      </c>
+      <c r="E12" t="s">
+        <v>271</v>
+      </c>
+      <c r="F12" t="s">
+        <v>272</v>
+      </c>
+      <c r="G12">
+        <v>231</v>
+      </c>
+      <c r="H12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>263</v>
+      </c>
+      <c r="B13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D13">
+        <v>2018</v>
+      </c>
+      <c r="E13" t="s">
+        <v>267</v>
+      </c>
+      <c r="F13" t="s">
+        <v>246</v>
+      </c>
+      <c r="G13">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>268</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>LEN(TRIM(C1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2614,7 +3129,7 @@
       <c r="Q1" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="7" t="s">
         <v>160</v>
       </c>
       <c r="S1" s="6" t="s">

</xml_diff>